<commit_message>
Updated ITA model - 2025-07-30 09:27
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SysSettings.xlsx
+++ b/VerveStacks_ITA/SysSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B00EC2B-AB19-4797-832A-DF4DEFB292AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAF95A2-FCFC-43CD-8D05-DD583126D455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="223">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -686,6 +686,27 @@
   </si>
   <si>
     <t>ITA</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>ELC_Sol-ITA</t>
+  </si>
+  <si>
+    <t>DAYNITE</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>Solar electricity produced in - Italy</t>
+  </si>
+  <si>
+    <t>ELC_Win-ITA</t>
+  </si>
+  <si>
+    <t>Wind electricity produced in - Italy</t>
   </si>
 </sst>
 </file>
@@ -3086,7 +3107,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F298A9-BCD9-4ABF-BE3B-9D1BDD3E7001}">
-  <dimension ref="B3:I20"/>
+  <dimension ref="B3:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -3104,7 +3125,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="17.649999999999999" thickBot="1">
+    <row r="3" spans="2:18" ht="17.649999999999999" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3116,7 +3137,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" ht="15" thickTop="1" thickBot="1">
+    <row r="4" spans="2:18" ht="15" thickTop="1" thickBot="1">
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3141,8 +3162,23 @@
       <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -3152,16 +3188,52 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="M5">
+        <v>249</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" t="s">
+        <v>217</v>
+      </c>
+      <c r="P5" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>219</v>
+      </c>
+      <c r="R5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18">
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="M6">
+        <v>253</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
+        <v>221</v>
+      </c>
+      <c r="P6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>219</v>
+      </c>
+      <c r="R6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -3169,7 +3241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:18">
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -3177,7 +3249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:18">
       <c r="C9" t="s">
         <v>24</v>
       </c>
@@ -3185,7 +3257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:18">
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -3193,7 +3265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:18">
       <c r="C11" t="s">
         <v>25</v>
       </c>
@@ -3201,7 +3273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:18">
       <c r="C12" t="s">
         <v>28</v>
       </c>
@@ -3209,7 +3281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:18">
       <c r="C13" t="s">
         <v>26</v>
       </c>
@@ -3217,7 +3289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:18">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -3225,7 +3297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:18">
       <c r="C15" t="s">
         <v>29</v>
       </c>
@@ -3245,7 +3317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:18">
       <c r="B16" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 09:30
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SysSettings.xlsx
+++ b/VerveStacks_ITA/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAF95A2-FCFC-43CD-8D05-DD583126D455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAC2312-F4E1-435A-9031-4C8D53EEF470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system_settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="223">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -3107,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F298A9-BCD9-4ABF-BE3B-9D1BDD3E7001}">
-  <dimension ref="B3:R20"/>
+  <dimension ref="B3:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3125,7 +3125,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="17.649999999999999" thickBot="1">
+    <row r="3" spans="2:17" ht="17.649999999999999" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3136,8 +3136,15 @@
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:18" ht="15" thickTop="1" thickBot="1">
+      <c r="M3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="2:17" ht="15" thickTop="1" thickBot="1">
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3162,23 +3169,23 @@
       <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O4" t="s">
+      <c r="N4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="P4" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Q4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:18">
+    <row r="5" spans="2:17">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -3188,52 +3195,46 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="M5">
-        <v>249</v>
+      <c r="M5" t="s">
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="O5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q5" t="s">
-        <v>219</v>
-      </c>
-      <c r="R5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="2:18">
+    <row r="6" spans="2:17">
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="M6">
-        <v>253</v>
+      <c r="M6" t="s">
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>221</v>
       </c>
       <c r="O6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q6" t="s">
-        <v>219</v>
-      </c>
-      <c r="R6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="2:18">
+    <row r="7" spans="2:17">
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:18">
+    <row r="8" spans="2:17">
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:18">
+    <row r="9" spans="2:17">
       <c r="C9" t="s">
         <v>24</v>
       </c>
@@ -3257,7 +3258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:18">
+    <row r="10" spans="2:17">
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:18">
+    <row r="11" spans="2:17">
       <c r="C11" t="s">
         <v>25</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:18">
+    <row r="12" spans="2:17">
       <c r="C12" t="s">
         <v>28</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:18">
+    <row r="13" spans="2:17">
       <c r="C13" t="s">
         <v>26</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="2:17">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="2:17">
       <c r="C15" t="s">
         <v>29</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="2:17">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -3686,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A64C410-895F-4040-A7AB-3F7211AA7FBD}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated BRA model - 2025-09-05 16:31
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SysSettings.xlsx
+++ b/VerveStacks_ITA/SysSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C3B125-B580-4421-90ED-58840D122214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81476550-080D-4357-9DFD-0DD89161B9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="221">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -100,12 +100,6 @@
     <t>bioenergy</t>
   </si>
   <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
     <t>hydrogen</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>solar</t>
   </si>
   <si>
-    <t>oil</t>
-  </si>
-  <si>
     <t>ELC</t>
   </si>
   <si>
@@ -670,9 +661,6 @@
     <t>windoff</t>
   </si>
   <si>
-    <t>NRG, GAS</t>
-  </si>
-  <si>
     <t>wind onshore</t>
   </si>
   <si>
@@ -704,6 +692,15 @@
   </si>
   <si>
     <t>onshore wind electricity generation</t>
+  </si>
+  <si>
+    <t>GAS</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>OIL</t>
   </si>
 </sst>
 </file>
@@ -3097,21 +3094,21 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:8">
       <c r="F5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3125,7 +3122,7 @@
   <dimension ref="B3:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3185,7 +3182,7 @@
         <v>16</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>10</v>
@@ -3217,19 +3214,19 @@
         <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:18">
@@ -3237,7 +3234,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -3246,27 +3243,27 @@
         <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="P6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -3275,19 +3272,19 @@
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="O7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="2:18">
@@ -3295,7 +3292,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -3306,7 +3303,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -3317,7 +3314,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -3328,7 +3325,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
@@ -3339,7 +3336,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>220</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
@@ -3350,7 +3347,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -3361,10 +3358,10 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -3375,10 +3372,10 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -3389,33 +3386,33 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -3423,13 +3420,13 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -3437,13 +3434,13 @@
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
@@ -3451,13 +3448,13 @@
     </row>
     <row r="20" spans="2:7">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
@@ -3468,55 +3465,55 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" t="s">
         <v>196</v>
-      </c>
-      <c r="C22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" t="s">
-        <v>198</v>
-      </c>
-      <c r="E22" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" t="s">
         <v>196</v>
-      </c>
-      <c r="C23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" t="s">
         <v>196</v>
-      </c>
-      <c r="C24" t="s">
-        <v>204</v>
-      </c>
-      <c r="E24" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3546,7 +3543,7 @@
   <sheetData>
     <row r="3" spans="2:7">
       <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -3556,28 +3553,28 @@
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="14.25">
       <c r="B12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="E12" s="8" t="str">
         <f>"msy"&amp;COUNT(E14:E46)&amp;"_"&amp;MAX(E14:E46)</f>
@@ -3597,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="14.25">
@@ -3605,7 +3602,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" ref="E14:G14" si="1">$B$4</f>
@@ -3625,7 +3622,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="6">
         <f>E14+3</f>
@@ -3645,7 +3642,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6">
         <f>E15+5</f>
@@ -3665,7 +3662,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" ref="E17:E20" si="2">E16+5</f>
@@ -3685,7 +3682,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="2"/>
@@ -3705,7 +3702,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="2"/>
@@ -3721,7 +3718,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="2"/>
@@ -3733,7 +3730,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="14.25">
@@ -3741,7 +3738,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="14.25">
@@ -3749,7 +3746,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="14.25">
@@ -3757,37 +3754,37 @@
         <v>10</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="14.25">
       <c r="B25" s="9"/>
       <c r="D25" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="14.25">
       <c r="B26" s="9"/>
       <c r="D26" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="14.25">
       <c r="B27" s="9"/>
       <c r="D27" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="14.25">
       <c r="B28" s="9"/>
       <c r="D28" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="14.25">
       <c r="B29" s="9"/>
       <c r="D29" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="14.25">
@@ -3861,7 +3858,7 @@
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3869,42 +3866,42 @@
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="J5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="L5" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="D6" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="11">
         <v>0</v>
@@ -3915,7 +3912,7 @@
     </row>
     <row r="7" spans="2:12">
       <c r="D7" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E7" s="11">
         <v>0</v>
@@ -3926,7 +3923,7 @@
     </row>
     <row r="8" spans="2:12">
       <c r="D8" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -3937,7 +3934,7 @@
     </row>
     <row r="9" spans="2:12">
       <c r="D9" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -3948,7 +3945,7 @@
     </row>
     <row r="10" spans="2:12">
       <c r="D10" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -3959,7 +3956,7 @@
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -3967,50 +3964,50 @@
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="D15" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="11">
         <v>2222</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="D16" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="11">
         <v>8888</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="12.75">
@@ -4412,13 +4409,13 @@
     <row r="2" spans="1:14" ht="17.649999999999999" thickBot="1">
       <c r="A2" s="13"/>
       <c r="B2" s="20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -4426,56 +4423,56 @@
     <row r="3" spans="1:14" ht="15" thickTop="1" thickBot="1">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I3" s="4">
         <v>2022</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13.15">
       <c r="A4" s="13"/>
       <c r="B4" s="19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="6"/>
       <c r="F4" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I4" s="11">
         <v>0.05</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N4" s="6">
         <v>1055.55</v>
@@ -4484,25 +4481,25 @@
     <row r="5" spans="1:14" ht="13.15">
       <c r="A5" s="13"/>
       <c r="B5" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I5" s="11">
         <v>1</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N5" s="6">
         <v>3.6</v>
@@ -4511,19 +4508,19 @@
     <row r="6" spans="1:14" ht="13.15">
       <c r="A6" s="13"/>
       <c r="B6" s="19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I6" s="11">
         <v>2025</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N6" s="6">
         <v>1000</v>
@@ -4532,19 +4529,19 @@
     <row r="7" spans="1:14" ht="13.15">
       <c r="A7" s="13"/>
       <c r="B7" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I7" s="11">
         <v>1</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N7" s="6">
         <v>1000</v>
@@ -4553,25 +4550,25 @@
     <row r="8" spans="1:14" ht="13.15">
       <c r="A8" s="13"/>
       <c r="B8" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I8" s="11">
         <v>2.2201</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N8" s="6">
         <v>1.05555</v>
@@ -4580,25 +4577,25 @@
     <row r="9" spans="1:14" ht="13.15">
       <c r="A9" s="13"/>
       <c r="B9" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I9" s="11">
         <v>2.1427</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N9" s="6">
         <v>4.1868000000000002E-2</v>
@@ -4607,25 +4604,25 @@
     <row r="10" spans="1:14" ht="13.15">
       <c r="A10" s="13"/>
       <c r="B10" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I10" s="11">
         <v>2.077</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N10" s="6">
         <v>41.868000000000002</v>
@@ -4634,25 +4631,25 @@
     <row r="11" spans="1:14" ht="13.15">
       <c r="A11" s="13"/>
       <c r="B11" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I11" s="11">
         <v>2.0358000000000001</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N11" s="6">
         <v>3.5999999999999999E-3</v>
@@ -4661,25 +4658,25 @@
     <row r="12" spans="1:14" ht="13.15">
       <c r="A12" s="13"/>
       <c r="B12" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I12" s="11">
         <v>1.9870000000000001</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N12" s="6">
         <v>1000000</v>
@@ -4688,25 +4685,25 @@
     <row r="13" spans="1:14" ht="13.15">
       <c r="A13" s="13"/>
       <c r="B13" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I13" s="11">
         <v>1.9192</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N13" s="6">
         <v>1000</v>
@@ -4715,25 +4712,25 @@
     <row r="14" spans="1:14" ht="13.15">
       <c r="A14" s="13"/>
       <c r="B14" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I14" s="11">
         <v>1.8468</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N14" s="6">
         <v>5.8615199999999996</v>
@@ -4742,25 +4739,25 @@
     <row r="15" spans="1:14" ht="13.15">
       <c r="A15" s="13"/>
       <c r="B15" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I15" s="11">
         <v>1.7799</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N15" s="6">
         <v>1E-3</v>
@@ -4769,25 +4766,25 @@
     <row r="16" spans="1:14" ht="13.15">
       <c r="A16" s="13"/>
       <c r="B16" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I16" s="11">
         <v>1.722</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N16" s="6">
         <v>1000</v>
@@ -4796,25 +4793,25 @@
     <row r="17" spans="1:14" ht="13.15">
       <c r="A17" s="13"/>
       <c r="B17" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I17" s="11">
         <v>1.6836</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N17" s="6">
         <v>37.68</v>
@@ -4822,25 +4819,25 @@
     </row>
     <row r="18" spans="1:14" ht="13.15">
       <c r="B18" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I18" s="11">
         <v>1.6446000000000001</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N18" s="6">
         <v>2139.4548</v>
@@ -4848,25 +4845,25 @@
     </row>
     <row r="19" spans="1:14" ht="13.15">
       <c r="B19" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I19" s="11">
         <v>1.6102000000000001</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N19" s="6">
         <v>2.78</v>
@@ -4874,25 +4871,25 @@
     </row>
     <row r="20" spans="1:14" ht="13.15">
       <c r="B20" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I20" s="11">
         <v>1.5770999999999999</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N20" s="6">
         <v>3.6</v>
@@ -4900,25 +4897,25 @@
     </row>
     <row r="21" spans="1:14" ht="13.15">
       <c r="B21" s="19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I21" s="11">
         <v>1.5488</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N21" s="6">
         <v>1</v>
@@ -4926,25 +4923,25 @@
     </row>
     <row r="22" spans="1:14" ht="13.15">
       <c r="B22" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I22" s="11">
         <v>1.5224</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N22" s="6">
         <v>31.536000000000001</v>
@@ -4952,25 +4949,25 @@
     </row>
     <row r="23" spans="1:14" ht="13.15">
       <c r="B23" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I23" s="11">
         <v>1.5058</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N23" s="6">
         <v>120</v>
@@ -4978,25 +4975,25 @@
     </row>
     <row r="24" spans="1:14" ht="13.15">
       <c r="B24" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I24" s="11">
         <v>1.4844999999999999</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N24" s="11">
         <v>5.8615199999999996</v>
@@ -5004,25 +5001,25 @@
     </row>
     <row r="25" spans="1:14" ht="13.15">
       <c r="B25" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I25" s="11">
         <v>1.4518</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N25" s="11">
         <v>54</v>
@@ -5030,16 +5027,16 @@
     </row>
     <row r="26" spans="1:14" ht="13.15">
       <c r="B26" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I26" s="11">
         <v>1.4198999999999999</v>
@@ -5047,16 +5044,16 @@
     </row>
     <row r="27" spans="1:14" ht="13.15">
       <c r="B27" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I27" s="11">
         <v>1.3986000000000001</v>
@@ -5064,16 +5061,16 @@
     </row>
     <row r="28" spans="1:14" ht="13.15">
       <c r="B28" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I28" s="11">
         <v>1.3727</v>
@@ -5081,16 +5078,16 @@
     </row>
     <row r="29" spans="1:14" ht="13.15">
       <c r="B29" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G29" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="H29" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I29" s="11">
         <v>1.3369</v>
@@ -5098,16 +5095,16 @@
     </row>
     <row r="30" spans="1:14" ht="13.15">
       <c r="B30" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I30" s="11">
         <v>1.2967</v>
@@ -5115,16 +5112,16 @@
     </row>
     <row r="31" spans="1:14" ht="13.15">
       <c r="B31" s="19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I31" s="11">
         <v>1.2583</v>
@@ -5132,16 +5129,16 @@
     </row>
     <row r="32" spans="1:14" ht="13.15">
       <c r="B32" s="19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I32" s="11">
         <v>1.2253000000000001</v>
@@ -5149,16 +5146,16 @@
     </row>
     <row r="33" spans="2:9" ht="13.15">
       <c r="B33" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I33" s="11">
         <v>1.2023999999999999</v>
@@ -5166,16 +5163,16 @@
     </row>
     <row r="34" spans="2:9" ht="13.15">
       <c r="B34" s="19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I34" s="11">
         <v>1.1931</v>
@@ -5183,16 +5180,16 @@
     </row>
     <row r="35" spans="2:9" ht="13.15">
       <c r="B35" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I35" s="11">
         <v>1.1793</v>
@@ -5200,16 +5197,16 @@
     </row>
     <row r="36" spans="2:9" ht="13.15">
       <c r="B36" s="19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I36" s="11">
         <v>1.1552</v>
@@ -5217,16 +5214,16 @@
     </row>
     <row r="37" spans="2:9" ht="13.15">
       <c r="B37" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I37" s="11">
         <v>1.1334</v>
@@ -5234,16 +5231,16 @@
     </row>
     <row r="38" spans="2:9" ht="13.15">
       <c r="B38" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I38" s="11">
         <v>1.1136999999999999</v>
@@ -5251,16 +5248,16 @@
     </row>
     <row r="39" spans="2:9" ht="13.15">
       <c r="B39" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I39" s="11">
         <v>1.0934999999999999</v>
@@ -5268,16 +5265,16 @@
     </row>
     <row r="40" spans="2:9" ht="13.15">
       <c r="B40" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I40" s="11">
         <v>1.0831</v>
@@ -5285,16 +5282,16 @@
     </row>
     <row r="41" spans="2:9" ht="13.15">
       <c r="B41" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I41" s="11">
         <v>1.0719000000000001</v>
@@ -5302,16 +5299,16 @@
     </row>
     <row r="42" spans="2:9" ht="13.15">
       <c r="B42" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I42" s="11">
         <v>1.0519000000000001</v>
@@ -5319,16 +5316,16 @@
     </row>
     <row r="43" spans="2:9" ht="13.15">
       <c r="B43" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I43" s="11">
         <v>1.0274000000000001</v>
@@ -5336,16 +5333,16 @@
     </row>
     <row r="44" spans="2:9" ht="13.15">
       <c r="B44" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I44" s="11">
         <v>1.0091000000000001</v>
@@ -5353,16 +5350,16 @@
     </row>
     <row r="45" spans="2:9" ht="13.15">
       <c r="B45" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I45" s="11">
         <v>1</v>
@@ -5370,16 +5367,16 @@
     </row>
     <row r="46" spans="2:9" ht="13.15">
       <c r="B46" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I46" s="11">
         <v>0.98960000000000004</v>
@@ -5387,16 +5384,16 @@
     </row>
     <row r="47" spans="2:9" ht="13.15">
       <c r="B47" s="19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I47" s="11">
         <v>0.97809999999999997</v>
@@ -5404,16 +5401,16 @@
     </row>
     <row r="48" spans="2:9" ht="13.15">
       <c r="B48" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I48" s="11">
         <v>0.96499999999999997</v>
@@ -5421,16 +5418,16 @@
     </row>
     <row r="49" spans="2:9" ht="13.15">
       <c r="B49" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I49" s="11">
         <v>0.94910000000000005</v>
@@ -5438,16 +5435,16 @@
     </row>
     <row r="50" spans="2:9" ht="13.15">
       <c r="B50" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I50" s="11">
         <v>0.92969999999999997</v>
@@ -5455,7 +5452,7 @@
     </row>
     <row r="51" spans="2:9" ht="13.15">
       <c r="B51" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F51" s="11" t="str">
         <f>F46</f>
@@ -5466,7 +5463,7 @@
         <v>USD20</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I51" s="11">
         <f t="shared" si="0"/>
@@ -5475,13 +5472,13 @@
     </row>
     <row r="52" spans="2:9" ht="13.15">
       <c r="B52" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I52" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5489,13 +5486,13 @@
     </row>
     <row r="53" spans="2:9" ht="13.15">
       <c r="B53" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I53" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5503,13 +5500,13 @@
     </row>
     <row r="54" spans="2:9" ht="13.15">
       <c r="B54" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I54" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5517,10 +5514,10 @@
     </row>
     <row r="55" spans="2:9">
       <c r="F55" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I55" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5528,10 +5525,10 @@
     </row>
     <row r="56" spans="2:9">
       <c r="F56" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I56" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5539,10 +5536,10 @@
     </row>
     <row r="57" spans="2:9">
       <c r="F57" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I57" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5550,10 +5547,10 @@
     </row>
     <row r="58" spans="2:9">
       <c r="F58" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I58" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5561,10 +5558,10 @@
     </row>
     <row r="59" spans="2:9">
       <c r="F59" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I59" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5572,10 +5569,10 @@
     </row>
     <row r="60" spans="2:9">
       <c r="F60" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I60" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5583,10 +5580,10 @@
     </row>
     <row r="61" spans="2:9">
       <c r="F61" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I61" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5594,10 +5591,10 @@
     </row>
     <row r="62" spans="2:9">
       <c r="F62" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I62" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5605,10 +5602,10 @@
     </row>
     <row r="63" spans="2:9">
       <c r="F63" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I63" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5616,10 +5613,10 @@
     </row>
     <row r="64" spans="2:9">
       <c r="F64" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I64" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5627,10 +5624,10 @@
     </row>
     <row r="65" spans="6:9">
       <c r="F65" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I65" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5638,10 +5635,10 @@
     </row>
     <row r="66" spans="6:9">
       <c r="F66" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I66" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5649,10 +5646,10 @@
     </row>
     <row r="67" spans="6:9">
       <c r="F67" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I67" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5660,10 +5657,10 @@
     </row>
     <row r="68" spans="6:9">
       <c r="F68" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I68" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5671,10 +5668,10 @@
     </row>
     <row r="69" spans="6:9">
       <c r="F69" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I69" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5682,10 +5679,10 @@
     </row>
     <row r="70" spans="6:9">
       <c r="F70" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I70" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5693,10 +5690,10 @@
     </row>
     <row r="71" spans="6:9">
       <c r="F71" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I71" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5704,10 +5701,10 @@
     </row>
     <row r="72" spans="6:9">
       <c r="F72" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I72" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5715,10 +5712,10 @@
     </row>
     <row r="73" spans="6:9">
       <c r="F73" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I73" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5726,10 +5723,10 @@
     </row>
     <row r="74" spans="6:9">
       <c r="F74" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I74" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5737,10 +5734,10 @@
     </row>
     <row r="75" spans="6:9">
       <c r="F75" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I75" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5748,10 +5745,10 @@
     </row>
     <row r="76" spans="6:9">
       <c r="F76" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I76" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5759,10 +5756,10 @@
     </row>
     <row r="77" spans="6:9">
       <c r="F77" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I77" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5770,10 +5767,10 @@
     </row>
     <row r="78" spans="6:9">
       <c r="F78" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I78" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5781,10 +5778,10 @@
     </row>
     <row r="79" spans="6:9">
       <c r="F79" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I79" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5792,10 +5789,10 @@
     </row>
     <row r="80" spans="6:9">
       <c r="F80" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I80" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5803,10 +5800,10 @@
     </row>
     <row r="81" spans="6:9">
       <c r="F81" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I81" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5814,10 +5811,10 @@
     </row>
     <row r="82" spans="6:9">
       <c r="F82" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I82" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5825,10 +5822,10 @@
     </row>
     <row r="83" spans="6:9">
       <c r="F83" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I83" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5836,10 +5833,10 @@
     </row>
     <row r="84" spans="6:9">
       <c r="F84" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I84" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5847,10 +5844,10 @@
     </row>
     <row r="85" spans="6:9">
       <c r="F85" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I85" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5858,10 +5855,10 @@
     </row>
     <row r="86" spans="6:9">
       <c r="F86" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I86" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5869,10 +5866,10 @@
     </row>
     <row r="87" spans="6:9">
       <c r="F87" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I87" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5880,10 +5877,10 @@
     </row>
     <row r="88" spans="6:9">
       <c r="F88" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I88" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5891,10 +5888,10 @@
     </row>
     <row r="89" spans="6:9">
       <c r="F89" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I89" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5902,10 +5899,10 @@
     </row>
     <row r="90" spans="6:9">
       <c r="F90" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I90" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5913,10 +5910,10 @@
     </row>
     <row r="91" spans="6:9">
       <c r="F91" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I91" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5924,10 +5921,10 @@
     </row>
     <row r="92" spans="6:9">
       <c r="F92" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I92" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5935,10 +5932,10 @@
     </row>
     <row r="93" spans="6:9">
       <c r="F93" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I93" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5946,10 +5943,10 @@
     </row>
     <row r="94" spans="6:9">
       <c r="F94" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I94" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5957,7 +5954,7 @@
     </row>
     <row r="95" spans="6:9">
       <c r="F95" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H95" s="11" t="str">
         <f>H51</f>
@@ -5969,39 +5966,39 @@
     </row>
     <row r="99" spans="5:10" ht="17.649999999999999" thickBot="1">
       <c r="E99" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="5:10" ht="15" thickTop="1" thickBot="1">
       <c r="E100" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I100" s="4">
         <v>2022</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="5:10" ht="14.25">
       <c r="E101"/>
       <c r="F101" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G101" s="21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H101" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I101" s="22">
         <f>1.10926234054354*I40</f>
@@ -6011,11 +6008,11 @@
     <row r="102" spans="5:10" ht="14.25">
       <c r="E102"/>
       <c r="F102" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G102"/>
       <c r="H102" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I102" s="22">
         <f>I84</f>
@@ -6043,26 +6040,26 @@
   <sheetData>
     <row r="3" spans="2:4" ht="17.649999999999999" thickBot="1">
       <c r="B3" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" thickTop="1" thickBot="1">
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D5" s="6">
         <v>-1</v>
@@ -6070,10 +6067,10 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -6081,10 +6078,10 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -6092,10 +6089,10 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -6103,10 +6100,10 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -6114,10 +6111,10 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -6125,10 +6122,10 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -6136,10 +6133,10 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -6147,10 +6144,10 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -6158,10 +6155,10 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D14" s="6">
         <v>2</v>
@@ -6169,10 +6166,10 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -6180,10 +6177,10 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D16" s="16">
         <v>1.0000000000000001E-5</v>
@@ -6191,10 +6188,10 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D17" s="16">
         <v>1.0000000000000001E-5</v>
@@ -6202,10 +6199,10 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D18" s="16">
         <v>1.0000000000000001E-5</v>
@@ -6213,10 +6210,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D19" s="16">
         <v>1.0000000000000001E-5</v>
@@ -6224,10 +6221,10 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D20" s="17">
         <v>1</v>
@@ -6235,73 +6232,73 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="17.649999999999999" thickBot="1">
       <c r="B25" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="15" thickTop="1" thickBot="1">
       <c r="B26" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>